<commit_message>
Added timestructure in normalisation code plus some other small fixes
</commit_message>
<xml_diff>
--- a/01-nuSIM/11-Parameters/nuSTORM-TrfLineCmplx-Params-v1.0.xlsx
+++ b/01-nuSIM/11-Parameters/nuSTORM-TrfLineCmplx-Params-v1.0.xlsx
@@ -210,10 +210,10 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.23"/>
@@ -245,7 +245,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Added timestructure in normalisation code plus some other small fixes (#18)
Co-authored-by: Marvin Pfaff <marvin.pfaff@tum.de>
</commit_message>
<xml_diff>
--- a/01-nuSIM/11-Parameters/nuSTORM-TrfLineCmplx-Params-v1.0.xlsx
+++ b/01-nuSIM/11-Parameters/nuSTORM-TrfLineCmplx-Params-v1.0.xlsx
@@ -210,10 +210,10 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.23"/>
@@ -245,7 +245,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Removed smearing in NEI to not smear twice; introduced transfer line to BeamDir calculation; introduced muon momentum acceptance cut in Absorption; changed constant input to nuSTORMConst.py; changed muon acceptance to 16% like in Snowmass white paper; added transfer line angle to parameter file and adjusted in NEI to get it from file and not having it hard-coded.
</commit_message>
<xml_diff>
--- a/01-nuSIM/11-Parameters/nuSTORM-TrfLineCmplx-Params-v1.0.xlsx
+++ b/01-nuSIM/11-Parameters/nuSTORM-TrfLineCmplx-Params-v1.0.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -47,6 +47,15 @@
   </si>
   <si>
     <t xml:space="preserve">nuSIM-2021-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer line complex angle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TrfLineCmplxAng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">°</t>
   </si>
   <si>
     <t xml:space="preserve">Momentum acceptance</t>
@@ -207,13 +216,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6953125" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.23"/>
@@ -262,7 +271,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>10</v>
+        <v>8.5</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>11</v>
@@ -279,7 +288,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>14</v>
@@ -296,7 +305,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>25000</v>
+        <v>1</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>17</v>
@@ -313,7 +322,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>2</v>
+        <v>25000</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>20</v>
@@ -330,10 +339,10 @@
         <v>22</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>8</v>
@@ -341,24 +350,40 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="0" t="n">
+      <c r="E8" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="0" t="n">
         <v>10.5</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="D9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>